<commit_message>
updated all paths to pathlib, improved cli help texts, and fixed commands.save to display txt before saving
</commit_message>
<xml_diff>
--- a/screenerfetch/workbooks/test/test.xlsx
+++ b/screenerfetch/workbooks/test/test.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hobbies\IT\Programming\Python\Projects\screenerfetch\screenerfetch\workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hobbies\IT\Programming\Python\Projects\screenerfetch\screenerfetch\workbooks\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6631A6F6-5068-46DC-B286-2570ACFA0B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10B6112-004B-4425-A15C-7D5C7D6356CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10453" uniqueCount="3624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10458" uniqueCount="3627">
   <si>
     <t>Date</t>
   </si>
@@ -10892,6 +10893,15 @@
   </si>
   <si>
     <t>-4.75</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Intraday</t>
+  </si>
+  <si>
+    <t>Daily</t>
   </si>
 </sst>
 </file>
@@ -10945,7 +10955,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -10953,10 +10965,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -11262,19 +11274,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1041"/>
+  <dimension ref="A1:O1052"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1006" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1016" sqref="T1016"/>
+      <pane ySplit="1" topLeftCell="A1028" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1042" sqref="A1042:O1052"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11" bestFit="1" customWidth="1"/>
@@ -11289,7 +11298,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -60210,6 +60219,226 @@
       </c>
       <c r="O1041" s="4">
         <v>3402371</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1042" s="3"/>
+      <c r="B1042" s="4"/>
+      <c r="C1042" s="4"/>
+      <c r="D1042" s="4"/>
+      <c r="E1042" s="4"/>
+      <c r="F1042" s="4"/>
+      <c r="G1042" s="4"/>
+      <c r="H1042" s="4"/>
+      <c r="I1042" s="4"/>
+      <c r="J1042" s="4"/>
+      <c r="K1042" s="4"/>
+      <c r="L1042" s="4"/>
+      <c r="M1042" s="4"/>
+      <c r="N1042" s="4"/>
+      <c r="O1042" s="4"/>
+    </row>
+    <row r="1043" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1043" s="3"/>
+      <c r="B1043" s="4"/>
+      <c r="C1043" s="4"/>
+      <c r="D1043" s="4"/>
+      <c r="E1043" s="4"/>
+      <c r="F1043" s="4"/>
+      <c r="G1043" s="4"/>
+      <c r="H1043" s="4"/>
+      <c r="I1043" s="4"/>
+      <c r="J1043" s="4"/>
+      <c r="K1043" s="4"/>
+      <c r="L1043" s="4"/>
+      <c r="M1043" s="4"/>
+      <c r="N1043" s="4"/>
+      <c r="O1043" s="4"/>
+    </row>
+    <row r="1044" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1044" s="3"/>
+      <c r="B1044" s="4"/>
+      <c r="C1044" s="4"/>
+      <c r="D1044" s="4"/>
+      <c r="E1044" s="4"/>
+      <c r="F1044" s="4"/>
+      <c r="G1044" s="4"/>
+      <c r="H1044" s="4"/>
+      <c r="I1044" s="4"/>
+      <c r="J1044" s="4"/>
+      <c r="K1044" s="4"/>
+      <c r="L1044" s="4"/>
+      <c r="M1044" s="4"/>
+      <c r="N1044" s="4"/>
+      <c r="O1044" s="4"/>
+    </row>
+    <row r="1045" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1045" s="3"/>
+      <c r="B1045" s="4"/>
+      <c r="C1045" s="4"/>
+      <c r="D1045" s="4"/>
+      <c r="E1045" s="4"/>
+      <c r="F1045" s="4"/>
+      <c r="G1045" s="4"/>
+      <c r="H1045" s="4"/>
+      <c r="I1045" s="4"/>
+      <c r="J1045" s="4"/>
+      <c r="K1045" s="4"/>
+      <c r="L1045" s="4"/>
+      <c r="M1045" s="4"/>
+      <c r="N1045" s="4"/>
+      <c r="O1045" s="4"/>
+    </row>
+    <row r="1046" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1046" s="3"/>
+      <c r="B1046" s="4"/>
+      <c r="C1046" s="4"/>
+      <c r="D1046" s="4"/>
+      <c r="E1046" s="4"/>
+      <c r="F1046" s="4"/>
+      <c r="G1046" s="4"/>
+      <c r="H1046" s="4"/>
+      <c r="I1046" s="4"/>
+      <c r="J1046" s="4"/>
+      <c r="K1046" s="4"/>
+      <c r="L1046" s="4"/>
+      <c r="M1046" s="4"/>
+      <c r="N1046" s="4"/>
+      <c r="O1046" s="4"/>
+    </row>
+    <row r="1047" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1047" s="3"/>
+      <c r="B1047" s="4"/>
+      <c r="C1047" s="4"/>
+      <c r="D1047" s="4"/>
+      <c r="E1047" s="4"/>
+      <c r="F1047" s="4"/>
+      <c r="G1047" s="4"/>
+      <c r="H1047" s="4"/>
+      <c r="I1047" s="4"/>
+      <c r="J1047" s="4"/>
+      <c r="K1047" s="4"/>
+      <c r="L1047" s="4"/>
+      <c r="M1047" s="4"/>
+      <c r="N1047" s="4"/>
+      <c r="O1047" s="4"/>
+    </row>
+    <row r="1048" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1048" s="3"/>
+      <c r="B1048" s="4"/>
+      <c r="C1048" s="4"/>
+      <c r="D1048" s="4"/>
+      <c r="E1048" s="4"/>
+      <c r="F1048" s="4"/>
+      <c r="G1048" s="4"/>
+      <c r="H1048" s="4"/>
+      <c r="I1048" s="4"/>
+      <c r="J1048" s="4"/>
+      <c r="K1048" s="4"/>
+      <c r="L1048" s="4"/>
+      <c r="M1048" s="4"/>
+      <c r="N1048" s="4"/>
+      <c r="O1048" s="4"/>
+    </row>
+    <row r="1049" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1049" s="3"/>
+      <c r="B1049" s="4"/>
+      <c r="C1049" s="4"/>
+      <c r="D1049" s="4"/>
+      <c r="E1049" s="4"/>
+      <c r="F1049" s="4"/>
+      <c r="G1049" s="4"/>
+      <c r="H1049" s="4"/>
+      <c r="I1049" s="4"/>
+      <c r="J1049" s="4"/>
+      <c r="K1049" s="4"/>
+      <c r="L1049" s="4"/>
+      <c r="M1049" s="4"/>
+      <c r="N1049" s="4"/>
+      <c r="O1049" s="4"/>
+    </row>
+    <row r="1050" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1050" s="3"/>
+      <c r="B1050" s="4"/>
+      <c r="C1050" s="4"/>
+      <c r="D1050" s="4"/>
+      <c r="E1050" s="4"/>
+      <c r="F1050" s="4"/>
+      <c r="G1050" s="4"/>
+      <c r="H1050" s="4"/>
+      <c r="I1050" s="4"/>
+      <c r="J1050" s="4"/>
+      <c r="K1050" s="4"/>
+      <c r="L1050" s="4"/>
+      <c r="M1050" s="4"/>
+      <c r="N1050" s="4"/>
+      <c r="O1050" s="4"/>
+    </row>
+    <row r="1051" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1051" s="3"/>
+      <c r="B1051" s="4"/>
+      <c r="C1051" s="4"/>
+      <c r="D1051" s="4"/>
+      <c r="E1051" s="4"/>
+      <c r="F1051" s="4"/>
+      <c r="G1051" s="4"/>
+      <c r="H1051" s="4"/>
+      <c r="I1051" s="4"/>
+      <c r="J1051" s="4"/>
+      <c r="K1051" s="4"/>
+      <c r="L1051" s="4"/>
+      <c r="M1051" s="4"/>
+      <c r="N1051" s="4"/>
+      <c r="O1051" s="4"/>
+    </row>
+    <row r="1052" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1052" s="3"/>
+      <c r="B1052" s="4"/>
+      <c r="C1052" s="4"/>
+      <c r="D1052" s="4"/>
+      <c r="E1052" s="4"/>
+      <c r="F1052" s="4"/>
+      <c r="G1052" s="4"/>
+      <c r="H1052" s="4"/>
+      <c r="I1052" s="4"/>
+      <c r="J1052" s="4"/>
+      <c r="K1052" s="4"/>
+      <c r="L1052" s="4"/>
+      <c r="M1052" s="4"/>
+      <c r="N1052" s="4"/>
+      <c r="O1052" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3624</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3625</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>